<commit_message>
Updating? Actually lost and confused
</commit_message>
<xml_diff>
--- a/Docs/CM_inventory.xlsx
+++ b/Docs/CM_inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6089-103_ATCA_mezz\GitHub\CU_PCB_6089-103\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{DA045487-8479-4CF9-80C3-08CC127F87B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{35E9C5C0-5041-8642-B553-B307E9831031}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BB7065-3EFE-4445-AD35-5A5CEC1D0873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="3195" windowWidth="21600" windowHeight="11415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Serial #</t>
   </si>
@@ -143,9 +143,6 @@
     <t>KU15P x12 14G FireFly (long)</t>
   </si>
   <si>
-    <t>W231</t>
-  </si>
-  <si>
     <t>sent to BU</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>TIF</t>
   </si>
   <si>
-    <t>broken power supply, was intended for use at TIF</t>
-  </si>
-  <si>
     <t>mated to SM 09</t>
   </si>
   <si>
@@ -170,9 +164,6 @@
     <t>bare board</t>
   </si>
   <si>
-    <t>socketed VU7P, no optics</t>
-  </si>
-  <si>
     <t>Major Location</t>
   </si>
   <si>
@@ -188,19 +179,16 @@
     <t>PSB ATCA crate</t>
   </si>
   <si>
-    <t>PSB Peter's lab</t>
-  </si>
-  <si>
-    <t>Peter's house</t>
-  </si>
-  <si>
-    <t>Peter's House</t>
-  </si>
-  <si>
     <t>mated to SM 10</t>
   </si>
   <si>
     <t>sent to TIF Oct 27, 2019. Mated to SM05.</t>
+  </si>
+  <si>
+    <t>Charlie's house</t>
+  </si>
+  <si>
+    <t>Rui's house</t>
   </si>
 </sst>
 </file>
@@ -555,28 +543,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.4140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.01171875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.28125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.02734375" style="5" customWidth="1"/>
-    <col min="5" max="6" width="10.76171875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9.14453125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.33984375" style="5" customWidth="1"/>
-    <col min="10" max="12" width="11.43359375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11" style="5" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="5" customWidth="1"/>
+    <col min="10" max="12" width="11.42578125" style="5" customWidth="1"/>
     <col min="13" max="13" width="2.28515625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="9.14453125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="16.94921875" customWidth="1"/>
-    <col min="16" max="16" width="55.5546875" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
+    <col min="16" max="16" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -611,16 +599,16 @@
         <v>34</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -631,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -655,16 +643,16 @@
         <v>0</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -682,7 +670,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -690,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
         <v>0</v>
@@ -717,16 +705,16 @@
         <v>0</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O4" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="P4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -744,7 +732,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -779,16 +767,16 @@
         <v>1</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O6" t="s">
         <v>51</v>
       </c>
       <c r="P6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -806,15 +794,15 @@
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5">
         <v>0</v>
@@ -841,16 +829,16 @@
         <v>0</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="P8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -868,7 +856,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -906,10 +894,10 @@
         <v>16</v>
       </c>
       <c r="P10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -927,7 +915,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -965,10 +953,10 @@
         <v>16</v>
       </c>
       <c r="P12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -986,7 +974,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1021,16 +1009,16 @@
         <v>0</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1048,7 +1036,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1083,16 +1071,16 @@
         <v>0</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1110,7 +1098,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1145,16 +1133,16 @@
         <v>0</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1172,7 +1160,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1210,10 +1198,10 @@
         <v>16</v>
       </c>
       <c r="P20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1231,21 +1219,21 @@
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="1:16" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="5">
         <f>SUM(B2:B21)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="5">
         <f>SUM(C2:C21)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D22" s="5">
         <f>SUM(D2:D21)</f>
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E22" s="5">
         <f>SUM(E2:E21)</f>
@@ -1276,7 +1264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="2" customFormat="1" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -1302,13 +1290,13 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="26" spans="1:16" s="11" customFormat="1" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="5">
         <f>D22</f>
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C26" s="5">
         <f>J22</f>
@@ -1316,7 +1304,7 @@
       </c>
       <c r="D26" s="5">
         <f>E26-(B26+C26)</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E26" s="5">
         <v>75</v>
@@ -1331,7 +1319,7 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1347,7 +1335,7 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:16" s="11" customFormat="1" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1378,7 +1366,7 @@
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1394,7 +1382,7 @@
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="1:16" s="11" customFormat="1" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1425,7 +1413,7 @@
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1441,18 +1429,18 @@
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="5">
         <f>B22+C22</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5">
         <f>E32-B32</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" s="5">
         <v>8</v>
@@ -1467,7 +1455,7 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1483,7 +1471,7 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="1:14" s="11" customFormat="1" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
@@ -1500,7 +1488,7 @@
         <v>7</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>

</xml_diff>